<commit_message>
gitignore updated for ignoring keys
</commit_message>
<xml_diff>
--- a/Plan for POC.xlsx
+++ b/Plan for POC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>R&amp;D</t>
   </si>
@@ -116,9 +116,6 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>Weight</t>
-  </si>
-  <si>
     <t>Alexa sample implementation</t>
   </si>
   <si>
@@ -168,13 +165,210 @@
   </si>
   <si>
     <t>Database structure</t>
+  </si>
+  <si>
+    <t>grocerymanagemntcosmosdb -&gt;grocerymanagemnt-database -&gt; grocerymanagemnt-collection</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">{ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB30000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"id"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"1"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB30000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"category"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Grocery"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB30000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"name"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"wheat"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB30000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"description"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"for roti"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>, "quantity":"1","specification":"kg",</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFB30000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"isComplete"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF07704A"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>false</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> }</t>
+    </r>
+  </si>
+  <si>
+    <t>Specification</t>
+  </si>
+  <si>
+    <t>IsComplete</t>
+  </si>
+  <si>
+    <t>{ "id": "2", "category": "Grocery", "name": "jaggery", "description": "brown color soft jaggery", "quantity":"1","specification":"kg","isComplete": false }</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,6 +397,30 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFB30000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFA31515"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF07704A"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -249,21 +467,23 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
+      <left style="thin">
         <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      </left>
+      <right style="thin">
         <color indexed="64"/>
-      </bottom>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -273,7 +493,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -287,8 +507,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -572,10 +793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L50"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27:G31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,30 +810,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="2">
+        <v>43221</v>
+      </c>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="2">
         <v>43221</v>
@@ -621,332 +857,300 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="2">
-        <v>43221</v>
-      </c>
-      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-    </row>
-    <row r="14" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+    </row>
+    <row r="9" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="2">
+        <v>43226</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="2">
+        <v>43226</v>
+      </c>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="2">
+        <v>43226</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="2">
-        <v>43226</v>
-      </c>
-      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2</v>
-      </c>
-      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>6</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>9</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>10</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>11</v>
+      </c>
+      <c r="B26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>12</v>
+      </c>
+      <c r="B27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>13</v>
+      </c>
+      <c r="B28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>14</v>
+      </c>
+      <c r="B29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>15</v>
+      </c>
+      <c r="B30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>16</v>
+      </c>
+      <c r="B31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="2">
-        <v>43226</v>
-      </c>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43">
         <v>1</v>
       </c>
-      <c r="B17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>2</v>
-      </c>
-      <c r="B18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="2">
-        <v>43226</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>3</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>4</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>5</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>6</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="4"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>4</v>
-      </c>
-      <c r="B25" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>5</v>
-      </c>
-      <c r="B26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>6</v>
-      </c>
-      <c r="B27" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>7</v>
-      </c>
-      <c r="B28" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>8</v>
-      </c>
-      <c r="B29" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>9</v>
-      </c>
-      <c r="B30" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>10</v>
-      </c>
-      <c r="B31" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>11</v>
-      </c>
-      <c r="B32" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>12</v>
-      </c>
-      <c r="B33" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>13</v>
-      </c>
-      <c r="B34" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>14</v>
-      </c>
-      <c r="B35" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>15</v>
-      </c>
-      <c r="B36" t="s">
-        <v>25</v>
-      </c>
-      <c r="C36" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>16</v>
-      </c>
-      <c r="B37" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
-      <c r="K39" s="10"/>
-      <c r="L39" s="10"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+      <c r="B43" t="s">
         <v>38</v>
       </c>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-      <c r="K48" s="1"/>
-      <c r="L48" s="1"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>1</v>
-      </c>
-      <c r="B50" t="s">
-        <v>39</v>
-      </c>
-      <c r="C50" t="s">
-        <v>33</v>
+      <c r="C43" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1016,45 +1220,65 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:D8"/>
+  <dimension ref="C2:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="13" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D4" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D5" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D6" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D7" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="G7" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D8" s="6" t="s">
-        <v>31</v>
+        <v>50</v>
+      </c>
+      <c r="G8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D9" s="11" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Grocery 13 May work Part 1
</commit_message>
<xml_diff>
--- a/Plan for POC.xlsx
+++ b/Plan for POC.xlsx
@@ -29,9 +29,6 @@
     <t>AWS Alexa R&amp;D</t>
   </si>
   <si>
-    <t>Xamarin forms list display</t>
-  </si>
-  <si>
     <t>Add category</t>
   </si>
   <si>
@@ -362,6 +359,9 @@
   </si>
   <si>
     <t>{ "id": "2", "category": "Grocery", "name": "jaggery", "description": "brown color soft jaggery", "quantity":"1","specification":"kg","isComplete": false }</t>
+  </si>
+  <si>
+    <t>ASP.NET Core Web API help pages with Swagger / Open API [Swashbuckle/Nswag = I used Nswag]</t>
   </si>
 </sst>
 </file>
@@ -793,15 +793,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="54.42578125" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" customWidth="1"/>
@@ -833,7 +833,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D2" s="2">
         <v>43221</v>
@@ -845,22 +845,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="D3" s="2">
         <v>43221</v>
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>2</v>
+      <c r="B4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="2">
+        <v>43233</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -868,7 +871,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -876,7 +879,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -884,49 +887,34 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-    </row>
-    <row r="9" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+    </row>
+    <row r="10" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>1</v>
       </c>
-      <c r="B9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="2">
-        <v>43226</v>
-      </c>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>2</v>
-      </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" s="2">
         <v>43226</v>
@@ -934,227 +922,243 @@
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="2">
+        <v>43226</v>
+      </c>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>39</v>
-      </c>
+      <c r="A12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="2">
-        <v>43226</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>3</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>33</v>
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="2">
+        <v>43226</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>5</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B17" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="19" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>6</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>7</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>9</v>
+      </c>
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>10</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>11</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>12</v>
+      </c>
+      <c r="B28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>13</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>14</v>
+      </c>
+      <c r="B30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>15</v>
+      </c>
+      <c r="B31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>4</v>
-      </c>
-      <c r="B19" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>5</v>
-      </c>
-      <c r="B20" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>6</v>
-      </c>
-      <c r="B21" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>7</v>
-      </c>
-      <c r="B22" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>8</v>
-      </c>
-      <c r="B23" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>9</v>
-      </c>
-      <c r="B24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>10</v>
-      </c>
-      <c r="B25" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>11</v>
-      </c>
-      <c r="B26" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>12</v>
-      </c>
-      <c r="B27" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>13</v>
-      </c>
-      <c r="B28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>14</v>
-      </c>
-      <c r="B29" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>15</v>
-      </c>
-      <c r="B30" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>16</v>
+      </c>
+      <c r="B32" t="s">
         <v>25</v>
       </c>
-      <c r="C30" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>16</v>
-      </c>
-      <c r="B31" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
-      <c r="J32" s="9"/>
-      <c r="K32" s="9"/>
-      <c r="L32" s="9"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44" t="s">
         <v>37</v>
       </c>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>1</v>
-      </c>
-      <c r="B43" t="s">
-        <v>38</v>
-      </c>
-      <c r="C43" t="s">
-        <v>32</v>
+      <c r="C44" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1182,10 +1186,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
         <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1193,10 +1197,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1204,10 +1208,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
         <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1233,48 +1237,48 @@
   <sheetData>
     <row r="2" spans="3:8" x14ac:dyDescent="0.25">
       <c r="H2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D4" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D5" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D6" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D7" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D8" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D9" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
can get list from cloud - 2 June 2018
</commit_message>
<xml_diff>
--- a/Plan for POC.xlsx
+++ b/Plan for POC.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
   <si>
     <t>R&amp;D</t>
   </si>
@@ -125,9 +125,6 @@
     <t>Project Infrastructure creation</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>Github source control integration</t>
   </si>
   <si>
@@ -362,6 +359,9 @@
   </si>
   <si>
     <t>ASP.NET Core Web API help pages with Swagger / Open API [Swashbuckle/Nswag = I used Nswag]</t>
+  </si>
+  <si>
+    <t>Publish .net core service on azure</t>
   </si>
 </sst>
 </file>
@@ -793,10 +793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,7 +860,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D4" s="2">
         <v>43233</v>
@@ -926,7 +926,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
         <v>31</v>
@@ -937,222 +937,237 @@
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="2">
+        <v>43253</v>
+      </c>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
-        <v>38</v>
-      </c>
+      <c r="A13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="2">
-        <v>43226</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>3</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>32</v>
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="2">
+        <v>43253</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>6</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>4</v>
-      </c>
-      <c r="B20" t="s">
-        <v>2</v>
-      </c>
+      <c r="B19" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B31" t="s">
-        <v>24</v>
-      </c>
-      <c r="C31" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
+        <v>15</v>
+      </c>
+      <c r="B32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>16</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-      <c r="J33" s="9"/>
-      <c r="K33" s="9"/>
-      <c r="L33" s="9"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="9"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="B45" t="s">
         <v>36</v>
       </c>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
-      <c r="L42" s="1"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>1</v>
-      </c>
-      <c r="B44" t="s">
-        <v>37</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1237,12 +1252,12 @@
   <sheetData>
     <row r="2" spans="3:8" x14ac:dyDescent="0.25">
       <c r="H2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="3:8" x14ac:dyDescent="0.25">
@@ -1265,20 +1280,20 @@
         <v>29</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D8" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D9" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>